<commit_message>
cedulas procesadas la noche de 1/10/2025
</commit_message>
<xml_diff>
--- a/cedulas.xlsx
+++ b/cedulas.xlsx
@@ -40,14 +40,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FF0000"/>
-        <bgColor rgb="00FF0000"/>
+        <fgColor rgb="0000FF00"/>
+        <bgColor rgb="0000FF00"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="0000FF00"/>
-        <bgColor rgb="0000FF00"/>
+        <fgColor rgb="00FF0000"/>
+        <bgColor rgb="00FF0000"/>
       </patternFill>
     </fill>
   </fills>
@@ -64,7 +64,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -412,1461 +413,1071 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:A290"/>
+  <dimension ref="A2:A212"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A259" workbookViewId="0">
-      <selection activeCell="A266" sqref="A266"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" outlineLevelCol="0"/>
   <cols>
-    <col width="26.7265625" customWidth="1" min="1" max="1"/>
-    <col width="21.08984375" customWidth="1" min="2" max="2"/>
-    <col width="17.81640625" customWidth="1" min="3" max="3"/>
+    <col width="26.7265625" customWidth="1" style="1" min="1" max="1"/>
+    <col width="21.08984375" customWidth="1" style="1" min="2" max="2"/>
+    <col width="17.81640625" customWidth="1" style="1" min="3" max="3"/>
   </cols>
   <sheetData>
     <row r="2">
-      <c r="A2" s="1" t="n">
+      <c r="A2" s="2" t="n">
         <v>30080356</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="n">
-        <v>21236224</v>
+      <c r="A3" s="3" t="n">
+        <v>21229026</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>21229026</v>
+      <c r="A4" s="3" t="n">
+        <v>39727147</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>39727147</v>
+      <c r="A5" s="3" t="n">
+        <v>17329021</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>17329021</v>
+      <c r="A6" s="3" t="n">
+        <v>39728361</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>39728361</v>
+      <c r="A7" s="2" t="n">
+        <v>40367231</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>40367231</v>
+      <c r="A8" s="3" t="n">
+        <v>37671025</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>37671025</v>
+      <c r="A9" s="2" t="n">
+        <v>40188151</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="2" t="n">
-        <v>30080371</v>
+      <c r="A10" s="3" t="n">
+        <v>40334977</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="n">
-        <v>40188151</v>
+      <c r="A11" s="2" t="n">
+        <v>1120498000</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="n">
-        <v>40334977</v>
+      <c r="A12" s="2" t="n">
+        <v>40403787</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="1" t="n">
-        <v>1120498000</v>
+      <c r="A13" s="2" t="n">
+        <v>1121891980</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="1" t="n">
-        <v>40403787</v>
+      <c r="A14" s="2" t="n">
+        <v>1121864632</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="1" t="n">
-        <v>1121891980</v>
+      <c r="A15" s="2" t="n">
+        <v>40332711</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="1" t="n">
-        <v>1121864632</v>
+      <c r="A16" s="2" t="n">
+        <v>1121847839</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="1" t="n">
-        <v>40332711</v>
+      <c r="A17" s="3" t="n">
+        <v>40413367</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>52655858</v>
+        <v>39648983</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
-        <v>1069900532</v>
+        <v>1007702703</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="1" t="n">
-        <v>1121847839</v>
+      <c r="A20" s="3" t="n">
+        <v>40218053</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
-        <v>40413127</v>
+        <v>1006442026</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="1" t="n">
-        <v>40413367</v>
+      <c r="A22" s="3" t="n">
+        <v>1121892958</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="1" t="n">
-        <v>39648983</v>
+      <c r="A23" s="2" t="n">
+        <v>1072395724</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="1" t="n">
-        <v>1007702703</v>
+      <c r="A24" s="2" t="n">
+        <v>1143252992</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
-        <v>1121857800</v>
+        <v>35261784</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="1" t="n">
-        <v>40218053</v>
+      <c r="A26" s="2" t="n">
+        <v>40394987</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="1" t="n">
-        <v>1006442026</v>
+      <c r="A27" s="2" t="n">
+        <v>40442006</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="n">
-        <v>1006774169</v>
+        <v>1001118801</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="n">
-        <v>1121906325</v>
+        <v>40390505</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="1" t="n">
-        <v>1121892958</v>
+      <c r="A30" s="2" t="n">
+        <v>1121955504</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="1" t="n">
-        <v>1072395724</v>
+      <c r="A31" s="2" t="n">
+        <v>1000832681</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="n">
-        <v>1121842098</v>
+        <v>1121849388</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="n">
-        <v>1121881992</v>
+        <v>1121818890</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="n">
-        <v>1121855560</v>
+        <v>1121954646</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="2" t="n">
-        <v>1001092252</v>
+      <c r="A35" s="3" t="n">
+        <v>21242719</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="1" t="n">
-        <v>1143252992</v>
+      <c r="A36" s="2" t="n">
+        <v>1121844971</v>
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="1" t="n">
-        <v>35261784</v>
+      <c r="A37" s="2" t="n">
+        <v>40215468</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="2" t="n">
-        <v>1121964736</v>
+        <v>1075277227</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="2" t="n">
-        <v>1006775869</v>
+        <v>1118291987</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="1" t="n">
-        <v>40394987</v>
+      <c r="A40" s="2" t="n">
+        <v>1121873859</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="2" t="n">
-        <v>1075685562</v>
+        <v>1121821756</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="1" t="n">
-        <v>40442006</v>
+      <c r="A42" s="2" t="n">
+        <v>1122653540</v>
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="1" t="n">
-        <v>1001118801</v>
+      <c r="A43" s="2" t="n">
+        <v>86086391</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="2" t="n">
-        <v>26163691</v>
+        <v>1006828058</v>
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="1" t="n">
-        <v>40390505</v>
+      <c r="A45" s="2" t="n">
+        <v>1121871447</v>
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="1" t="n">
-        <v>1121955504</v>
+      <c r="A46" s="2" t="n">
+        <v>40218016</v>
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="1" t="n">
-        <v>1000832681</v>
+      <c r="A47" s="2" t="n">
+        <v>1121917747</v>
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="1" t="n">
-        <v>1121849388</v>
+      <c r="A48" s="2" t="n">
+        <v>1121827017</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="2" t="n">
-        <v>1121944032</v>
+        <v>1121862649</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="2" t="n">
-        <v>1122652964</v>
+        <v>1006798198</v>
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="1" t="n">
-        <v>1121818890</v>
+      <c r="A51" s="3" t="n">
+        <v>1121852594</v>
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="1" t="n">
-        <v>1121954646</v>
+      <c r="A52" s="2" t="n">
+        <v>1121946818</v>
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="1" t="n">
-        <v>21242719</v>
+      <c r="A53" s="3" t="n">
+        <v>1125552959</v>
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="1" t="n">
-        <v>1121844971</v>
+      <c r="A54" s="2" t="n">
+        <v>40331222</v>
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="2" t="n">
-        <v>1006775707</v>
+      <c r="A55" s="3" t="n">
+        <v>1056782595</v>
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="1" t="n">
-        <v>40215468</v>
+      <c r="A56" s="2" t="n">
+        <v>1006772734</v>
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="1" t="n">
-        <v>1075277227</v>
+      <c r="A57" s="2" t="n">
+        <v>1121893657</v>
       </c>
     </row>
     <row r="58">
-      <c r="A58" t="n">
-        <v>1118291987</v>
+      <c r="A58" s="2" t="n">
+        <v>1121849200</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="2" t="n">
-        <v>40443728</v>
+        <v>1014184746</v>
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="1" t="n">
-        <v>1121873859</v>
+      <c r="A60" s="3" t="n">
+        <v>1023035549</v>
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="1" t="n">
-        <v>1121821756</v>
+      <c r="A61" s="3" t="n">
+        <v>1007413869</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="2" t="n">
-        <v>42031731</v>
+        <v>1006828141</v>
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="1" t="n">
-        <v>1122653540</v>
+      <c r="A63" s="3" t="n">
+        <v>1122138078</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="2" t="n">
-        <v>30083822</v>
+        <v>1121896390</v>
       </c>
     </row>
     <row r="65">
-      <c r="A65" s="1" t="n">
-        <v>86086391</v>
+      <c r="A65" s="3" t="n">
+        <v>40401474</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="2" t="n">
-        <v>40394841</v>
+        <v>1121824236</v>
       </c>
     </row>
     <row r="67">
-      <c r="A67" s="1" t="n">
-        <v>1006828058</v>
+      <c r="A67" s="2" t="n">
+        <v>1123561577</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="2" t="n">
-        <v>1121960138</v>
+        <v>40325807</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="2" t="n">
-        <v>40334349</v>
+        <v>40441092</v>
       </c>
     </row>
     <row r="70">
-      <c r="A70" s="2" t="n">
-        <v>20851383</v>
+      <c r="A70" s="3" t="n">
+        <v>38290869</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="2" t="n">
-        <v>1121836742</v>
+        <v>1123801589</v>
       </c>
     </row>
     <row r="72">
-      <c r="A72" s="1" t="n">
-        <v>1121871447</v>
+      <c r="A72" s="2" t="n">
+        <v>1127391633</v>
       </c>
     </row>
     <row r="73">
-      <c r="A73" s="2" t="n">
-        <v>1007228432</v>
+      <c r="A73" s="3" t="n">
+        <v>40386471</v>
       </c>
     </row>
     <row r="74">
-      <c r="A74" s="1" t="n">
-        <v>40218016</v>
+      <c r="A74" s="2" t="n">
+        <v>1030623737</v>
       </c>
     </row>
     <row r="75">
-      <c r="A75" s="2" t="n">
-        <v>1121824999</v>
+      <c r="A75" s="3" t="n">
+        <v>40388244</v>
       </c>
     </row>
     <row r="76">
-      <c r="A76" s="1" t="n">
-        <v>1121917747</v>
+      <c r="A76" s="2" t="n">
+        <v>52977026</v>
       </c>
     </row>
     <row r="77">
-      <c r="A77" s="1" t="n">
-        <v>1121827017</v>
+      <c r="A77" s="2" t="n">
+        <v>52862750</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="2" t="n">
-        <v>1057574560</v>
+        <v>1007741689</v>
       </c>
     </row>
     <row r="79">
-      <c r="A79" s="1" t="n">
-        <v>1121862649</v>
+      <c r="A79" s="2" t="n">
+        <v>40189602</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="2" t="n">
-        <v>40217183</v>
+        <v>1234790567</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="2" t="n">
-        <v>40325663</v>
+        <v>1006335084</v>
       </c>
     </row>
     <row r="82">
-      <c r="A82" s="1" t="n">
-        <v>1006798198</v>
+      <c r="A82" s="2" t="n">
+        <v>1234789507</v>
       </c>
     </row>
     <row r="83">
-      <c r="A83" s="1" t="n">
-        <v>1121852594</v>
+      <c r="A83" s="2" t="n">
+        <v>1033748818</v>
       </c>
     </row>
     <row r="84">
-      <c r="A84" s="1" t="n">
-        <v>1121946818</v>
+      <c r="A84" s="3" t="n">
+        <v>1121946821</v>
       </c>
     </row>
     <row r="85">
-      <c r="A85" s="1" t="n">
-        <v>1125552959</v>
+      <c r="A85" s="2" t="n">
+        <v>1121915532</v>
       </c>
     </row>
     <row r="86">
-      <c r="A86" s="1" t="n">
-        <v>40331222</v>
+      <c r="A86" s="2" t="n">
+        <v>1120378354</v>
       </c>
     </row>
     <row r="87">
-      <c r="A87" s="1" t="n">
-        <v>1056782595</v>
+      <c r="A87" s="3" t="n">
+        <v>1007816099</v>
       </c>
     </row>
     <row r="88">
-      <c r="A88" s="1" t="n">
-        <v>1006772734</v>
+      <c r="A88" s="2" t="n">
+        <v>1005566462</v>
       </c>
     </row>
     <row r="89">
-      <c r="A89" s="1" t="n">
-        <v>1121893657</v>
+      <c r="A89" s="2" t="n">
+        <v>1005294945</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="2" t="n">
-        <v>1193092381</v>
+        <v>1122655308</v>
       </c>
     </row>
     <row r="91">
-      <c r="A91" s="1" t="n">
-        <v>1121849200</v>
+      <c r="A91" s="2" t="n">
+        <v>1006775023</v>
       </c>
     </row>
     <row r="92">
-      <c r="A92" s="2" t="n">
-        <v>1012331970</v>
+      <c r="A92" s="3" t="n">
+        <v>1006797846</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="2" t="n">
-        <v>1012342436</v>
+        <v>1003583504</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="2" t="n">
-        <v>1121853595</v>
+        <v>1121146010</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="2" t="n">
-        <v>35587282</v>
+        <v>1122653301</v>
       </c>
     </row>
     <row r="96">
-      <c r="A96" s="1" t="n">
-        <v>1014184746</v>
+      <c r="A96" s="2" t="n">
+        <v>40186992</v>
       </c>
     </row>
     <row r="97">
-      <c r="A97" s="1" t="n">
-        <v>1023035549</v>
+      <c r="A97" s="2" t="n">
+        <v>1010123626</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="2" t="n">
-        <v>40326656</v>
+        <v>1234789441</v>
       </c>
     </row>
     <row r="99">
-      <c r="A99" s="1" t="n">
-        <v>1007413869</v>
+      <c r="A99" s="2" t="n">
+        <v>1123431666</v>
       </c>
     </row>
     <row r="100">
-      <c r="A100" s="1" t="n">
-        <v>1006828141</v>
+      <c r="A100" s="2" t="n">
+        <v>1006859731</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="2" t="n">
-        <v>1121841888</v>
+        <v>1120385112</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="2" t="n">
-        <v>52619648</v>
+        <v>1121921356</v>
       </c>
     </row>
     <row r="103">
-      <c r="A103" s="1" t="n">
-        <v>1122138078</v>
+      <c r="A103" s="3" t="n">
+        <v>1006774144</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="2" t="n">
-        <v>40186281</v>
+        <v>1123140904</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="2" t="n">
-        <v>40371926</v>
+        <v>1010031875</v>
       </c>
     </row>
     <row r="106">
-      <c r="A106" s="1" t="n">
-        <v>1121896390</v>
+      <c r="A106" s="2" t="n">
+        <v>46376887</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="2" t="n">
-        <v>35261879</v>
+        <v>1006820624</v>
       </c>
     </row>
     <row r="108">
-      <c r="A108" s="1" t="n">
-        <v>40401474</v>
+      <c r="A108" s="2" t="n">
+        <v>1121833506</v>
       </c>
     </row>
     <row r="109">
-      <c r="A109" s="1" t="n">
-        <v>1121824236</v>
+      <c r="A109" s="2" t="n">
+        <v>1121888058</v>
       </c>
     </row>
     <row r="110">
-      <c r="A110" s="1" t="n">
-        <v>1123561577</v>
+      <c r="A110" s="2" t="n">
+        <v>1122919487</v>
       </c>
     </row>
     <row r="111">
-      <c r="A111" s="1" t="n">
-        <v>40325807</v>
+      <c r="A111" s="2" t="n">
+        <v>1193221023</v>
       </c>
     </row>
     <row r="112">
-      <c r="A112" s="1" t="n">
-        <v>40441092</v>
+      <c r="A112" s="3" t="n">
+        <v>1121872788</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="2" t="n">
-        <v>40188434</v>
+        <v>1069735886</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="2" t="n">
-        <v>40402375</v>
+        <v>1007437551</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="2" t="n">
-        <v>40444722</v>
+        <v>1121931106</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="2" t="n">
-        <v>1193557701</v>
+        <v>1014243158</v>
       </c>
     </row>
     <row r="117">
-      <c r="A117" s="1" t="n">
-        <v>38290869</v>
+      <c r="A117" s="2" t="n">
+        <v>1121944349</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="2" t="n">
-        <v>52205911</v>
+        <v>1000580172</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="2" t="n">
-        <v>21231994</v>
+        <v>1085280827</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="2" t="n">
-        <v>1121920906</v>
+        <v>1014292653</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="2" t="n">
-        <v>42548918</v>
+        <v>52710556</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="2" t="n">
-        <v>40441978</v>
+        <v>1121822749</v>
       </c>
     </row>
     <row r="123">
-      <c r="A123" s="1" t="n">
-        <v>1123801589</v>
+      <c r="A123" s="2" t="n">
+        <v>1001174715</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="2" t="n">
-        <v>1121817317</v>
+        <v>1123430278</v>
       </c>
     </row>
     <row r="125">
-      <c r="A125" s="1" t="n">
-        <v>1127391633</v>
+      <c r="A125" s="2" t="n">
+        <v>1022408192</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="2" t="n">
-        <v>1121915258</v>
+        <v>1121836926</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="2" t="n">
-        <v>1121899304</v>
+        <v>40333112</v>
       </c>
     </row>
     <row r="128">
-      <c r="A128" s="1" t="n">
-        <v>40386471</v>
+      <c r="A128" s="2" t="n">
+        <v>1127382143</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="2" t="n">
-        <v>1121925708</v>
+        <v>1002577155</v>
       </c>
     </row>
     <row r="130">
-      <c r="A130" s="2" t="n">
-        <v>1121846671</v>
+      <c r="A130" s="3" t="n">
+        <v>24100971</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="2" t="n">
-        <v>40400188</v>
+        <v>1002085841</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="2" t="n">
-        <v>1121968595</v>
+        <v>1121935079</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="2" t="n">
-        <v>1006874896</v>
+        <v>1006827679</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="2" t="n">
-        <v>51883053</v>
+        <v>1006736555</v>
       </c>
     </row>
     <row r="135">
-      <c r="A135" s="1" t="n">
-        <v>1030623737</v>
+      <c r="A135" s="2" t="n">
+        <v>1029982510</v>
       </c>
     </row>
     <row r="136">
-      <c r="A136" s="1" t="n">
-        <v>40388244</v>
+      <c r="A136" s="2" t="n">
+        <v>1001885026</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="2" t="n">
-        <v>37397372</v>
+        <v>1121960484</v>
       </c>
     </row>
     <row r="138">
-      <c r="A138" s="1" t="n">
-        <v>52977026</v>
+      <c r="A138" s="2" t="n">
+        <v>1007702953</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="2" t="n">
-        <v>40392197</v>
+        <v>1006722113</v>
       </c>
     </row>
     <row r="140">
-      <c r="A140" s="2" t="n">
-        <v>1121823721</v>
+      <c r="A140" s="3" t="n">
+        <v>1029981260</v>
       </c>
     </row>
     <row r="141">
-      <c r="A141" s="1" t="n">
-        <v>52862750</v>
+      <c r="A141" s="2" t="n">
+        <v>1007730620</v>
       </c>
     </row>
     <row r="142">
-      <c r="A142" s="1" t="n">
-        <v>1007741689</v>
+      <c r="A142" s="2" t="n">
+        <v>1007318395</v>
       </c>
     </row>
     <row r="143">
-      <c r="A143" s="1" t="n">
-        <v>40189602</v>
+      <c r="A143" s="2" t="n">
+        <v>1121923083</v>
       </c>
     </row>
     <row r="144">
-      <c r="A144" s="1" t="n">
-        <v>1234790567</v>
+      <c r="A144" s="2" t="n">
+        <v>1014306063</v>
       </c>
     </row>
     <row r="145">
-      <c r="A145" s="1" t="n">
-        <v>1006335084</v>
+      <c r="A145" t="n">
+        <v>1097990010</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="2" t="n">
-        <v>1121849738</v>
+        <v>1121919401</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="2" t="n">
-        <v>1099210766</v>
+        <v>1022341095</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="2" t="n">
-        <v>1121918538</v>
+        <v>1233490733</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="2" t="n">
-        <v>1116439136</v>
+        <v>1123803651</v>
       </c>
     </row>
     <row r="150">
-      <c r="A150" s="1" t="n">
-        <v>1234789507</v>
+      <c r="A150" s="2" t="n">
+        <v>39570143</v>
       </c>
     </row>
     <row r="151">
-      <c r="A151" t="n">
-        <v>1033748818</v>
+      <c r="A151" s="3" t="n">
+        <v>1121849836</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" s="2" t="n">
-        <v>1121908839</v>
+        <v>1029982301</v>
       </c>
     </row>
     <row r="153">
-      <c r="A153" s="1" t="n">
-        <v>1121946821</v>
+      <c r="A153" s="2" t="n">
+        <v>52483077</v>
       </c>
     </row>
     <row r="154">
-      <c r="A154" s="1" t="n">
-        <v>1121915532</v>
+      <c r="A154" s="2" t="n">
+        <v>1121146397</v>
       </c>
     </row>
     <row r="155">
-      <c r="A155" s="1" t="n">
-        <v>1120378354</v>
+      <c r="A155" s="2" t="n">
+        <v>1006658626</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" s="2" t="n">
-        <v>1006835763</v>
+        <v>40439256</v>
       </c>
     </row>
     <row r="157">
-      <c r="A157" s="1" t="n">
-        <v>1007816099</v>
+      <c r="A157" s="3" t="n">
+        <v>52501176</v>
       </c>
     </row>
     <row r="158">
-      <c r="A158" s="1" t="n">
-        <v>1005566462</v>
+      <c r="A158" s="2" t="n">
+        <v>1121834547</v>
       </c>
     </row>
     <row r="159">
-      <c r="A159" s="1" t="n">
-        <v>1005294945</v>
+      <c r="A159" s="2" t="n">
+        <v>1122507401</v>
       </c>
     </row>
     <row r="160">
-      <c r="A160" s="1" t="n">
-        <v>1122655308</v>
+      <c r="A160" s="2" t="n">
+        <v>1121940276</v>
       </c>
     </row>
     <row r="161">
-      <c r="A161" t="n">
-        <v>1123561702</v>
+      <c r="A161" s="2" t="n">
+        <v>1122507035</v>
       </c>
     </row>
     <row r="162">
-      <c r="A162" t="n">
-        <v>1006775023</v>
+      <c r="A162" s="2" t="n">
+        <v>1013674750</v>
       </c>
     </row>
     <row r="163">
-      <c r="A163" t="n">
-        <v>1006797846</v>
+      <c r="A163" s="2" t="n">
+        <v>1122511768</v>
       </c>
     </row>
     <row r="164">
-      <c r="A164" t="n">
-        <v>1003583504</v>
+      <c r="A164" s="2" t="n">
+        <v>1122918696</v>
       </c>
     </row>
     <row r="165">
-      <c r="A165" t="n">
-        <v>1121146010</v>
+      <c r="A165" s="2" t="n">
+        <v>1120926035</v>
       </c>
     </row>
     <row r="166">
-      <c r="A166" t="n">
-        <v>1122653301</v>
+      <c r="A166" s="3" t="n">
+        <v>1121830619</v>
       </c>
     </row>
     <row r="167">
-      <c r="A167" t="n">
-        <v>1121879243</v>
+      <c r="A167" s="2" t="n">
+        <v>77777780</v>
       </c>
     </row>
     <row r="168">
-      <c r="A168" t="n">
-        <v>1120365722</v>
+      <c r="A168" s="2" t="n">
+        <v>1022960497</v>
       </c>
     </row>
     <row r="169">
-      <c r="A169" t="n">
-        <v>1121948797</v>
+      <c r="A169" s="2" t="n">
+        <v>1113692397</v>
       </c>
     </row>
     <row r="170">
-      <c r="A170" t="n">
-        <v>1120559199</v>
+      <c r="A170" s="2" t="n">
+        <v>1036840503</v>
       </c>
     </row>
     <row r="171">
-      <c r="A171" t="n">
-        <v>1006690427</v>
+      <c r="A171" s="2" t="n">
+        <v>1006695715</v>
       </c>
     </row>
     <row r="172">
-      <c r="A172" t="n">
-        <v>1121720012</v>
+      <c r="A172" s="2" t="n">
+        <v>63471947</v>
       </c>
     </row>
     <row r="173">
-      <c r="A173" t="n">
-        <v>1121961367</v>
+      <c r="A173" s="2" t="n">
+        <v>1121965996</v>
       </c>
     </row>
     <row r="174">
-      <c r="A174" t="n">
-        <v>40186992</v>
+      <c r="A174" s="2" t="n">
+        <v>1006692119</v>
       </c>
     </row>
     <row r="175">
-      <c r="A175" t="n">
-        <v>1010123626</v>
+      <c r="A175" s="2" t="n">
+        <v>1121931253</v>
       </c>
     </row>
     <row r="176">
-      <c r="A176" t="n">
-        <v>1234789441</v>
+      <c r="A176" s="2" t="n">
+        <v>40333161</v>
       </c>
     </row>
     <row r="177">
-      <c r="A177" t="n">
-        <v>1123431666</v>
+      <c r="A177" s="2" t="n">
+        <v>1120870248</v>
       </c>
     </row>
     <row r="178">
-      <c r="A178" t="n">
-        <v>1006859731</v>
+      <c r="A178" s="2" t="n">
+        <v>1120871550</v>
       </c>
     </row>
     <row r="179">
-      <c r="A179" t="n">
-        <v>1120385112</v>
+      <c r="A179" s="2" t="n">
+        <v>1123860010</v>
       </c>
     </row>
     <row r="180">
-      <c r="A180" t="n">
-        <v>1121921356</v>
+      <c r="A180" s="3" t="n">
+        <v>1077976735</v>
       </c>
     </row>
     <row r="181">
-      <c r="A181" t="n">
-        <v>1006774144</v>
+      <c r="A181" s="2" t="n">
+        <v>1234789628</v>
       </c>
     </row>
     <row r="182">
-      <c r="A182" t="n">
-        <v>1123140904</v>
+      <c r="A182" s="2" t="n">
+        <v>1065644681</v>
       </c>
     </row>
     <row r="183">
-      <c r="A183" t="n">
-        <v>1010031875</v>
+      <c r="A183" s="2" t="n">
+        <v>1006819843</v>
       </c>
     </row>
     <row r="184">
-      <c r="A184" t="n">
-        <v>46376887</v>
+      <c r="A184" s="3" t="n">
+        <v>1005159244</v>
       </c>
     </row>
     <row r="185">
-      <c r="A185" t="n">
-        <v>1006820624</v>
+      <c r="A185" s="3" t="n">
+        <v>1006794572</v>
       </c>
     </row>
     <row r="186">
-      <c r="A186" t="n">
-        <v>1121833506</v>
+      <c r="A186" s="3" t="n">
+        <v>1006824446</v>
       </c>
     </row>
     <row r="187">
-      <c r="A187" t="n">
-        <v>1121888058</v>
+      <c r="A187" s="2" t="n">
+        <v>1193092480</v>
       </c>
     </row>
     <row r="188">
-      <c r="A188" t="n">
-        <v>1122919487</v>
+      <c r="A188" s="3" t="n">
+        <v>1121915979</v>
       </c>
     </row>
     <row r="189">
-      <c r="A189" t="n">
-        <v>1193221023</v>
+      <c r="A189" s="2" t="n">
+        <v>1122647759</v>
       </c>
     </row>
     <row r="190">
-      <c r="A190" t="n">
-        <v>1121872788</v>
+      <c r="A190" s="2" t="n">
+        <v>1121874758</v>
       </c>
     </row>
     <row r="191">
-      <c r="A191" t="n">
-        <v>1069735886</v>
+      <c r="A191" s="2" t="n">
+        <v>1005848328</v>
       </c>
     </row>
     <row r="192">
-      <c r="A192" t="n">
-        <v>1007437551</v>
+      <c r="A192" s="2" t="n">
+        <v>1121416122</v>
       </c>
     </row>
     <row r="193">
-      <c r="A193" t="n">
-        <v>1121931106</v>
+      <c r="A193" s="2" t="n">
+        <v>1007584794</v>
       </c>
     </row>
     <row r="194">
-      <c r="A194" t="n">
-        <v>1014243158</v>
+      <c r="A194" s="2" t="n">
+        <v>1121927207</v>
       </c>
     </row>
     <row r="195">
-      <c r="A195" t="n">
-        <v>1121944349</v>
+      <c r="A195" s="2" t="n">
+        <v>1122918521</v>
       </c>
     </row>
     <row r="196">
-      <c r="A196" t="n">
-        <v>1000580172</v>
+      <c r="A196" s="2" t="n">
+        <v>1003565669</v>
       </c>
     </row>
     <row r="197">
-      <c r="A197" t="n">
-        <v>1085280827</v>
+      <c r="A197" s="2" t="n">
+        <v>1106775925</v>
       </c>
     </row>
     <row r="198">
-      <c r="A198" t="n">
-        <v>1014292653</v>
+      <c r="A198" s="2" t="n">
+        <v>1121966736</v>
       </c>
     </row>
     <row r="199">
-      <c r="A199" t="n">
-        <v>52710556</v>
+      <c r="A199" s="2" t="n">
+        <v>1121931564</v>
       </c>
     </row>
     <row r="200">
-      <c r="A200" t="n">
-        <v>1121822749</v>
+      <c r="A200" s="2" t="n">
+        <v>1121817727</v>
       </c>
     </row>
     <row r="201">
-      <c r="A201" t="n">
-        <v>1001174715</v>
+      <c r="A201" s="3" t="n">
+        <v>1022999589</v>
       </c>
     </row>
     <row r="202">
-      <c r="A202" t="n">
-        <v>1123430278</v>
+      <c r="A202" s="3" t="n">
+        <v>1006656639</v>
       </c>
     </row>
     <row r="203">
-      <c r="A203" t="n">
-        <v>1022408192</v>
+      <c r="A203" s="3" t="n">
+        <v>1096196072</v>
       </c>
     </row>
     <row r="204">
-      <c r="A204" t="n">
-        <v>1121836926</v>
+      <c r="A204" s="2" t="n">
+        <v>1122511568</v>
       </c>
     </row>
     <row r="205">
-      <c r="A205" t="n">
-        <v>40333112</v>
+      <c r="A205" s="2" t="n">
+        <v>1118532809</v>
       </c>
     </row>
     <row r="206">
-      <c r="A206" t="n">
-        <v>1127382143</v>
+      <c r="A206" s="2" t="n">
+        <v>1006796310</v>
       </c>
     </row>
     <row r="207">
-      <c r="A207" t="n">
-        <v>1002577155</v>
+      <c r="A207" s="2" t="n">
+        <v>53062799</v>
       </c>
     </row>
     <row r="208">
       <c r="A208" t="n">
-        <v>24100971</v>
+        <v>1106888062</v>
       </c>
     </row>
     <row r="209">
       <c r="A209" t="n">
-        <v>1002085841</v>
+        <v>1121844532</v>
       </c>
     </row>
     <row r="210">
       <c r="A210" t="n">
-        <v>1121935079</v>
+        <v>1034660761</v>
       </c>
     </row>
     <row r="211">
       <c r="A211" t="n">
-        <v>1006827679</v>
+        <v>1005848329</v>
       </c>
     </row>
     <row r="212">
       <c r="A212" t="n">
-        <v>1006736555</v>
-      </c>
-    </row>
-    <row r="213">
-      <c r="A213" t="n">
-        <v>1029982510</v>
-      </c>
-    </row>
-    <row r="214">
-      <c r="A214" t="n">
-        <v>1001885026</v>
-      </c>
-    </row>
-    <row r="215">
-      <c r="A215" t="n">
-        <v>1121960484</v>
-      </c>
-    </row>
-    <row r="216">
-      <c r="A216" t="n">
-        <v>1007702953</v>
-      </c>
-    </row>
-    <row r="217">
-      <c r="A217" t="n">
-        <v>1006722113</v>
-      </c>
-    </row>
-    <row r="218">
-      <c r="A218" t="n">
-        <v>1029981260</v>
-      </c>
-    </row>
-    <row r="219">
-      <c r="A219" t="n">
-        <v>1007730620</v>
-      </c>
-    </row>
-    <row r="220">
-      <c r="A220" t="n">
-        <v>1007318395</v>
-      </c>
-    </row>
-    <row r="221">
-      <c r="A221" t="n">
-        <v>1121923083</v>
-      </c>
-    </row>
-    <row r="222">
-      <c r="A222" t="n">
-        <v>1014306063</v>
-      </c>
-    </row>
-    <row r="223">
-      <c r="A223" t="n">
-        <v>1097990010</v>
-      </c>
-    </row>
-    <row r="224">
-      <c r="A224" t="n">
-        <v>1121919401</v>
-      </c>
-    </row>
-    <row r="225">
-      <c r="A225" t="n">
-        <v>1022341095</v>
-      </c>
-    </row>
-    <row r="226">
-      <c r="A226" t="n">
-        <v>1233490733</v>
-      </c>
-    </row>
-    <row r="227">
-      <c r="A227" t="n">
-        <v>1123803651</v>
-      </c>
-    </row>
-    <row r="228">
-      <c r="A228" t="n">
-        <v>39570143</v>
-      </c>
-    </row>
-    <row r="229">
-      <c r="A229" t="n">
-        <v>1121849836</v>
-      </c>
-    </row>
-    <row r="230">
-      <c r="A230" t="n">
-        <v>1029982301</v>
-      </c>
-    </row>
-    <row r="231">
-      <c r="A231" t="n">
-        <v>52483077</v>
-      </c>
-    </row>
-    <row r="232">
-      <c r="A232" t="n">
-        <v>1121146397</v>
-      </c>
-    </row>
-    <row r="233">
-      <c r="A233" t="n">
-        <v>1006658626</v>
-      </c>
-    </row>
-    <row r="234">
-      <c r="A234" t="n">
-        <v>40439256</v>
-      </c>
-    </row>
-    <row r="235">
-      <c r="A235" t="n">
-        <v>52501176</v>
-      </c>
-    </row>
-    <row r="236">
-      <c r="A236" t="n">
-        <v>1121834547</v>
-      </c>
-    </row>
-    <row r="237">
-      <c r="A237" t="n">
-        <v>1122507401</v>
-      </c>
-    </row>
-    <row r="238">
-      <c r="A238" t="n">
-        <v>1121940276</v>
-      </c>
-    </row>
-    <row r="239">
-      <c r="A239" t="n">
-        <v>1122507035</v>
-      </c>
-    </row>
-    <row r="240">
-      <c r="A240" t="n">
-        <v>1013674750</v>
-      </c>
-    </row>
-    <row r="241">
-      <c r="A241" t="n">
-        <v>1122511768</v>
-      </c>
-    </row>
-    <row r="242">
-      <c r="A242" t="n">
-        <v>1122918696</v>
-      </c>
-    </row>
-    <row r="243">
-      <c r="A243" t="n">
-        <v>1120926035</v>
-      </c>
-    </row>
-    <row r="244">
-      <c r="A244" t="n">
-        <v>1121830619</v>
-      </c>
-    </row>
-    <row r="245">
-      <c r="A245" t="n">
-        <v>77777780</v>
-      </c>
-    </row>
-    <row r="246">
-      <c r="A246" t="n">
-        <v>1022960497</v>
-      </c>
-    </row>
-    <row r="247">
-      <c r="A247" t="n">
-        <v>1113692397</v>
-      </c>
-    </row>
-    <row r="248">
-      <c r="A248" t="n">
-        <v>1036840503</v>
-      </c>
-    </row>
-    <row r="249">
-      <c r="A249" t="n">
-        <v>1006695715</v>
-      </c>
-    </row>
-    <row r="250">
-      <c r="A250" t="n">
-        <v>63471947</v>
-      </c>
-    </row>
-    <row r="251">
-      <c r="A251" t="n">
-        <v>1121965996</v>
-      </c>
-    </row>
-    <row r="252">
-      <c r="A252" t="n">
-        <v>1006692119</v>
-      </c>
-    </row>
-    <row r="253">
-      <c r="A253" t="n">
-        <v>1121931253</v>
-      </c>
-    </row>
-    <row r="254">
-      <c r="A254" t="n">
-        <v>40333161</v>
-      </c>
-    </row>
-    <row r="255">
-      <c r="A255" t="n">
-        <v>1120870248</v>
-      </c>
-    </row>
-    <row r="256">
-      <c r="A256" t="n">
-        <v>1120871550</v>
-      </c>
-    </row>
-    <row r="257">
-      <c r="A257" t="n">
-        <v>1123860010</v>
-      </c>
-    </row>
-    <row r="258">
-      <c r="A258" t="n">
-        <v>1077976735</v>
-      </c>
-    </row>
-    <row r="259">
-      <c r="A259" t="n">
-        <v>1234789628</v>
-      </c>
-    </row>
-    <row r="260">
-      <c r="A260" t="n">
-        <v>1065644681</v>
-      </c>
-    </row>
-    <row r="261">
-      <c r="A261" t="n">
-        <v>1006819843</v>
-      </c>
-    </row>
-    <row r="262">
-      <c r="A262" t="n">
-        <v>1005159244</v>
-      </c>
-    </row>
-    <row r="263">
-      <c r="A263" t="n">
-        <v>1006794572</v>
-      </c>
-    </row>
-    <row r="264">
-      <c r="A264" t="n">
-        <v>1006824446</v>
-      </c>
-    </row>
-    <row r="265">
-      <c r="A265" t="n">
-        <v>1193092480</v>
-      </c>
-    </row>
-    <row r="266">
-      <c r="A266" t="n">
-        <v>1121915979</v>
-      </c>
-    </row>
-    <row r="267">
-      <c r="A267" t="n">
-        <v>1122647759</v>
-      </c>
-    </row>
-    <row r="268">
-      <c r="A268" t="n">
-        <v>1121874758</v>
-      </c>
-    </row>
-    <row r="269">
-      <c r="A269" t="n">
-        <v>1005848328</v>
-      </c>
-    </row>
-    <row r="270">
-      <c r="A270" t="n">
-        <v>1121416122</v>
-      </c>
-    </row>
-    <row r="271">
-      <c r="A271" t="n">
-        <v>1007584794</v>
-      </c>
-    </row>
-    <row r="272">
-      <c r="A272" t="n">
-        <v>1121927207</v>
-      </c>
-    </row>
-    <row r="273">
-      <c r="A273" t="n">
-        <v>1122918521</v>
-      </c>
-    </row>
-    <row r="274">
-      <c r="A274" t="n">
-        <v>1003565669</v>
-      </c>
-    </row>
-    <row r="275">
-      <c r="A275" t="n">
-        <v>1106775925</v>
-      </c>
-    </row>
-    <row r="276">
-      <c r="A276" t="n">
-        <v>1121966736</v>
-      </c>
-    </row>
-    <row r="277">
-      <c r="A277" t="n">
-        <v>1121931564</v>
-      </c>
-    </row>
-    <row r="278">
-      <c r="A278" t="n">
-        <v>1121817727</v>
-      </c>
-    </row>
-    <row r="279">
-      <c r="A279" t="n">
-        <v>1022999589</v>
-      </c>
-    </row>
-    <row r="280">
-      <c r="A280" t="n">
-        <v>1006656639</v>
-      </c>
-    </row>
-    <row r="281">
-      <c r="A281" t="n">
-        <v>1096196072</v>
-      </c>
-    </row>
-    <row r="282">
-      <c r="A282" t="n">
-        <v>1122511568</v>
-      </c>
-    </row>
-    <row r="283">
-      <c r="A283" t="n">
-        <v>1118532809</v>
-      </c>
-    </row>
-    <row r="284">
-      <c r="A284" t="n">
-        <v>1006796310</v>
-      </c>
-    </row>
-    <row r="285">
-      <c r="A285" t="n">
-        <v>53062799</v>
-      </c>
-    </row>
-    <row r="286">
-      <c r="A286" t="n">
-        <v>1106888062</v>
-      </c>
-    </row>
-    <row r="287">
-      <c r="A287" t="n">
-        <v>1121844532</v>
-      </c>
-    </row>
-    <row r="288">
-      <c r="A288" t="n">
-        <v>1034660761</v>
-      </c>
-    </row>
-    <row r="289">
-      <c r="A289" t="n">
-        <v>1005848329</v>
-      </c>
-    </row>
-    <row r="290">
-      <c r="A290" t="n">
         <v>1121817958</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Cedulas pendientes por cerrar sesion x2
</commit_message>
<xml_diff>
--- a/cedulas.xlsx
+++ b/cedulas.xlsx
@@ -794,7 +794,7 @@
       </c>
     </row>
     <row r="74">
-      <c r="A74" t="n">
+      <c r="A74" s="2" t="n">
         <v>31006869</v>
       </c>
     </row>
@@ -804,47 +804,47 @@
       </c>
     </row>
     <row r="76">
-      <c r="A76" t="n">
+      <c r="A76" s="3" t="n">
         <v>40306131</v>
       </c>
     </row>
     <row r="77">
-      <c r="A77" t="n">
+      <c r="A77" s="2" t="n">
         <v>40422019</v>
       </c>
     </row>
     <row r="78">
-      <c r="A78" t="n">
+      <c r="A78" s="2" t="n">
         <v>1006697169</v>
       </c>
     </row>
     <row r="79">
-      <c r="A79" t="n">
+      <c r="A79" s="2" t="n">
         <v>1124216732</v>
       </c>
     </row>
     <row r="80">
-      <c r="A80" t="n">
+      <c r="A80" s="3" t="n">
         <v>1120355361</v>
       </c>
     </row>
     <row r="81">
-      <c r="A81" t="n">
+      <c r="A81" s="2" t="n">
         <v>30081386</v>
       </c>
     </row>
     <row r="82">
-      <c r="A82" t="n">
+      <c r="A82" s="3" t="n">
         <v>1122138895</v>
       </c>
     </row>
     <row r="83">
-      <c r="A83" t="n">
+      <c r="A83" s="2" t="n">
         <v>21940107</v>
       </c>
     </row>
     <row r="84">
-      <c r="A84" t="n">
+      <c r="A84" s="3" t="n">
         <v>40187078</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Cedulas pendientes por cerrar sesion x3
</commit_message>
<xml_diff>
--- a/cedulas.xlsx
+++ b/cedulas.xlsx
@@ -849,102 +849,102 @@
       </c>
     </row>
     <row r="85">
-      <c r="A85" t="n">
+      <c r="A85" s="2" t="n">
         <v>40433512</v>
       </c>
     </row>
     <row r="86">
-      <c r="A86" t="n">
+      <c r="A86" s="2" t="n">
         <v>18598661</v>
       </c>
     </row>
     <row r="87">
-      <c r="A87" t="n">
+      <c r="A87" s="2" t="n">
         <v>86009284</v>
       </c>
     </row>
     <row r="88">
-      <c r="A88" t="n">
+      <c r="A88" s="2" t="n">
         <v>31006780</v>
       </c>
     </row>
     <row r="89">
-      <c r="A89" t="n">
+      <c r="A89" s="2" t="n">
         <v>28845786</v>
       </c>
     </row>
     <row r="90">
-      <c r="A90" t="n">
+      <c r="A90" s="3" t="n">
         <v>1071304162</v>
       </c>
     </row>
     <row r="91">
-      <c r="A91" t="n">
+      <c r="A91" s="2" t="n">
         <v>1120373472</v>
       </c>
     </row>
     <row r="92">
-      <c r="A92" t="n">
+      <c r="A92" s="2" t="n">
         <v>14952515</v>
       </c>
     </row>
     <row r="93">
-      <c r="A93" t="n">
+      <c r="A93" s="3" t="n">
         <v>1104184087</v>
       </c>
     </row>
     <row r="94">
-      <c r="A94" t="n">
+      <c r="A94" s="2" t="n">
         <v>1098436557</v>
       </c>
     </row>
     <row r="95">
-      <c r="A95" t="n">
+      <c r="A95" s="3" t="n">
         <v>21182488</v>
       </c>
     </row>
     <row r="96">
-      <c r="A96" t="n">
+      <c r="A96" s="3" t="n">
         <v>1076200860</v>
       </c>
     </row>
     <row r="97">
-      <c r="A97" t="n">
+      <c r="A97" s="3" t="n">
         <v>1118562246</v>
       </c>
     </row>
     <row r="98">
-      <c r="A98" t="n">
+      <c r="A98" s="3" t="n">
         <v>1012413227</v>
       </c>
     </row>
     <row r="99">
-      <c r="A99" t="n">
+      <c r="A99" s="3" t="n">
         <v>1005181518</v>
       </c>
     </row>
     <row r="100">
-      <c r="A100" t="n">
+      <c r="A100" s="3" t="n">
         <v>1119887995</v>
       </c>
     </row>
     <row r="101">
-      <c r="A101" t="n">
+      <c r="A101" s="3" t="n">
         <v>1120369362</v>
       </c>
     </row>
     <row r="102">
-      <c r="A102" t="n">
+      <c r="A102" s="3" t="n">
         <v>1006777681</v>
       </c>
     </row>
     <row r="103">
-      <c r="A103" t="n">
+      <c r="A103" s="2" t="n">
         <v>80266280</v>
       </c>
     </row>
     <row r="104">
-      <c r="A104" t="n">
+      <c r="A104" s="3" t="n">
         <v>1120362791</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Cedulas pendientes por cerrar sesion x4
</commit_message>
<xml_diff>
--- a/cedulas.xlsx
+++ b/cedulas.xlsx
@@ -949,162 +949,162 @@
       </c>
     </row>
     <row r="105">
-      <c r="A105" t="n">
+      <c r="A105" s="3" t="n">
         <v>1111197763</v>
       </c>
     </row>
     <row r="106">
-      <c r="A106" t="n">
+      <c r="A106" s="2" t="n">
         <v>1121875236</v>
       </c>
     </row>
     <row r="107">
-      <c r="A107" t="n">
+      <c r="A107" s="3" t="n">
         <v>1122138809</v>
       </c>
     </row>
     <row r="108">
-      <c r="A108" t="n">
+      <c r="A108" s="2" t="n">
         <v>1123512956</v>
       </c>
     </row>
     <row r="109">
-      <c r="A109" t="n">
+      <c r="A109" s="3" t="n">
         <v>1121416747</v>
       </c>
     </row>
     <row r="110">
-      <c r="A110" t="n">
+      <c r="A110" s="3" t="n">
         <v>1120498474</v>
       </c>
     </row>
     <row r="111">
-      <c r="A111" t="n">
+      <c r="A111" s="3" t="n">
         <v>1123114456</v>
       </c>
     </row>
     <row r="112">
-      <c r="A112" t="n">
+      <c r="A112" s="3" t="n">
         <v>40405695</v>
       </c>
     </row>
     <row r="113">
-      <c r="A113" t="n">
+      <c r="A113" s="3" t="n">
         <v>1120372119</v>
       </c>
     </row>
     <row r="114">
-      <c r="A114" t="n">
+      <c r="A114" s="2" t="n">
         <v>1123114061</v>
       </c>
     </row>
     <row r="115">
-      <c r="A115" t="n">
+      <c r="A115" s="2" t="n">
         <v>1121903090</v>
       </c>
     </row>
     <row r="116">
-      <c r="A116" t="n">
+      <c r="A116" s="3" t="n">
         <v>1116505062</v>
       </c>
     </row>
     <row r="117">
-      <c r="A117" t="n">
+      <c r="A117" s="2" t="n">
         <v>1006697920</v>
       </c>
     </row>
     <row r="118">
-      <c r="A118" t="n">
+      <c r="A118" s="3" t="n">
         <v>40265478</v>
       </c>
     </row>
     <row r="119">
-      <c r="A119" t="n">
+      <c r="A119" s="2" t="n">
         <v>1123085348</v>
       </c>
     </row>
     <row r="120">
-      <c r="A120" t="n">
+      <c r="A120" s="2" t="n">
         <v>1120006623</v>
       </c>
     </row>
     <row r="121">
-      <c r="A121" t="n">
+      <c r="A121" s="2" t="n">
         <v>1122646404</v>
       </c>
     </row>
     <row r="122">
-      <c r="A122" t="n">
+      <c r="A122" s="3" t="n">
         <v>1056771673</v>
       </c>
     </row>
     <row r="123">
-      <c r="A123" t="n">
+      <c r="A123" s="2" t="n">
         <v>21991161</v>
       </c>
     </row>
     <row r="124">
-      <c r="A124" t="n">
+      <c r="A124" s="3" t="n">
         <v>40445242</v>
       </c>
     </row>
     <row r="125">
-      <c r="A125" t="n">
+      <c r="A125" s="2" t="n">
         <v>1120381379</v>
       </c>
     </row>
     <row r="126">
-      <c r="A126" t="n">
+      <c r="A126" s="2" t="n">
         <v>1121921932</v>
       </c>
     </row>
     <row r="127">
-      <c r="A127" t="n">
+      <c r="A127" s="3" t="n">
         <v>1000693714</v>
       </c>
     </row>
     <row r="128">
-      <c r="A128" t="n">
+      <c r="A128" s="3" t="n">
         <v>1005319257</v>
       </c>
     </row>
     <row r="129">
-      <c r="A129" t="n">
+      <c r="A129" s="3" t="n">
         <v>1193112708</v>
       </c>
     </row>
     <row r="130">
-      <c r="A130" t="n">
+      <c r="A130" s="3" t="n">
         <v>1120355934</v>
       </c>
     </row>
     <row r="131">
-      <c r="A131" t="n">
+      <c r="A131" s="3" t="n">
         <v>1016945097</v>
       </c>
     </row>
     <row r="132">
-      <c r="A132" t="n">
+      <c r="A132" s="3" t="n">
         <v>1006777121</v>
       </c>
     </row>
     <row r="133">
-      <c r="A133" t="n">
+      <c r="A133" s="3" t="n">
         <v>1121146244</v>
       </c>
     </row>
     <row r="134">
-      <c r="A134" t="n">
+      <c r="A134" s="3" t="n">
         <v>1123515171</v>
       </c>
     </row>
     <row r="135">
-      <c r="A135" t="n">
+      <c r="A135" s="2" t="n">
         <v>1006874253</v>
       </c>
     </row>
     <row r="136">
-      <c r="A136" t="n">
+      <c r="A136" s="2" t="n">
         <v>1123567290</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ejecucion de facturas de cerrar sesion
</commit_message>
<xml_diff>
--- a/cedulas.xlsx
+++ b/cedulas.xlsx
@@ -1,51 +1,74 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ContratosSuperflex\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB1829CD-6FB5-4DAF-9356-4A9404A98BE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="4">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <u val="single"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFFF0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0000FF00"/>
+        <bgColor rgb="0000FF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF0000"/>
+        <bgColor rgb="00FF0000"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -61,23 +84,88 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="7">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -343,412 +431,257 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:A80"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A2:C48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="26.77734375" customWidth="1"/>
-    <col min="2" max="2" width="21.109375" customWidth="1"/>
-    <col min="3" max="3" width="17.77734375" customWidth="1"/>
+    <col width="26.81640625" customWidth="1" min="1" max="1"/>
+    <col width="21.08984375" customWidth="1" min="2" max="2"/>
+    <col width="17.81640625" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>21229026</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>39727147</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>17329021</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>39728361</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>40334977</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>1125552959</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8">
+    <row r="2">
+      <c r="A2" s="4" t="n">
         <v>1023035549</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9">
+    <row r="3">
+      <c r="A3" s="4" t="n">
         <v>38290869</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>40386471</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11">
+    <row r="4">
+      <c r="A4" s="4" t="n">
         <v>1121946821</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>1007816099</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A13">
+    <row r="5">
+      <c r="A5" s="5" t="n">
         <v>1006797846</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A14">
+    <row r="6">
+      <c r="A6" s="4" t="n">
         <v>1006774144</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A15">
+    <row r="7">
+      <c r="A7" s="5" t="n">
         <v>1121872788</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <v>24100971</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <v>1029981260</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <v>1121830619</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19">
+    <row r="8">
+      <c r="A8" s="4" t="n">
         <v>1006794572</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20">
+    <row r="9">
+      <c r="A9" s="4" t="n">
         <v>1006824446</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21">
-        <v>1096196072</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22">
-        <v>1034660761</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23">
-        <v>21205258</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24">
-        <v>17360686</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A25">
-        <v>51642333</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A26">
-        <v>3292415</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27">
-        <v>11373533</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A28">
-        <v>30030456</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A29">
-        <v>70052315</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A30">
-        <v>3282146</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A31">
+    <row r="10">
+      <c r="A10" s="4" t="n">
         <v>3045925</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A32">
+    <row r="11">
+      <c r="A11" s="4" t="n">
         <v>21173140</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33">
+    <row r="12">
+      <c r="A12" s="4" t="n">
         <v>21234532</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34">
+    <row r="13">
+      <c r="A13" s="4" t="n">
         <v>6671921</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35">
+    <row r="14">
+      <c r="A14" s="4" t="n">
         <v>4561950</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A36">
+    <row r="15">
+      <c r="A15" s="4" t="n">
         <v>19337954</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A37">
+    <row r="16">
+      <c r="A16" s="4" t="n">
         <v>40434896</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A38">
-        <v>1123860656</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A39">
-        <v>30055352</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A40">
+    <row r="17">
+      <c r="A17" s="6" t="n">
         <v>59671136</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A41">
+    <row r="18">
+      <c r="A18" s="6" t="n">
         <v>21177991</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A42">
+    <row r="19">
+      <c r="A19" s="6" t="n">
         <v>14993451</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A43">
+      <c r="C19" s="3" t="n"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="6" t="n">
         <v>40361978</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A44">
+    <row r="21">
+      <c r="A21" s="6" t="n">
         <v>7818547</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A45">
-        <v>40412991</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A46">
+    <row r="22">
+      <c r="A22" s="6" t="n">
         <v>86040029</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A47">
+    <row r="23">
+      <c r="A23" s="4" t="n">
         <v>40265797</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A48">
+    <row r="24">
+      <c r="A24" s="4" t="n">
         <v>37559806</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A49">
+    <row r="25">
+      <c r="A25" s="4" t="n">
         <v>79849312</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A50">
-        <v>1121148787</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A51">
+    <row r="26">
+      <c r="A26" s="4" t="n">
         <v>1000807612</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A52">
+    <row r="27">
+      <c r="A27" s="4" t="n">
         <v>31006869</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A53">
-        <v>1124190027</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A54">
+    <row r="28">
+      <c r="A28" s="4" t="n">
         <v>40422019</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A55">
+    <row r="29">
+      <c r="A29" s="4" t="n">
         <v>1006697169</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A56">
-        <v>1124216732</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A57">
+    <row r="30">
+      <c r="A30" s="4" t="n">
         <v>30081386</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A58">
+    <row r="31">
+      <c r="A31" s="4" t="n">
         <v>21940107</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A59">
-        <v>40433512</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A60">
+    <row r="32">
+      <c r="A32" s="4" t="n">
         <v>18598661</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A61">
+    <row r="33">
+      <c r="A33" s="4" t="n">
         <v>86009284</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A62">
+    <row r="34">
+      <c r="A34" s="4" t="n">
         <v>31006780</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A63">
+    <row r="35">
+      <c r="A35" s="4" t="n">
         <v>28845786</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A64">
-        <v>1120373472</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A65">
+    <row r="36">
+      <c r="A36" s="4" t="n">
         <v>14952515</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A66">
-        <v>1098436557</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A67">
-        <v>80266280</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A68">
+    <row r="37">
+      <c r="A37" s="4" t="n">
         <v>1121875236</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A69">
+    <row r="38">
+      <c r="A38" s="4" t="n">
         <v>1123512956</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A70">
+    <row r="39">
+      <c r="A39" s="4" t="n">
         <v>1123114061</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A71">
+    <row r="40">
+      <c r="A40" s="4" t="n">
         <v>1121903090</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A72">
+    <row r="41">
+      <c r="A41" s="4" t="n">
         <v>1006697920</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A73">
+    <row r="42">
+      <c r="A42" s="4" t="n">
         <v>1123085348</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A74">
+    <row r="43">
+      <c r="A43" s="4" t="n">
         <v>1120006623</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A75">
+    <row r="44">
+      <c r="A44" s="4" t="n">
         <v>1122646404</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A76">
+    <row r="45">
+      <c r="A45" s="4" t="n">
         <v>21991161</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A77">
+    <row r="46">
+      <c r="A46" s="4" t="n">
         <v>1120381379</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A78">
+    <row r="47">
+      <c r="A47" s="4" t="n">
         <v>1121921932</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A79">
-        <v>1006874253</v>
-      </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A80">
+    <row r="48">
+      <c r="A48" s="4" t="n">
         <v>1123567290</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ultima ejecucion, sin cedulas remanentes
</commit_message>
<xml_diff>
--- a/cedulas.xlsx
+++ b/cedulas.xlsx
@@ -1,61 +1,62 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ContratosSuperflex\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15A249C9-4896-473B-AF6D-5870C9BFC484}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="4">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="11"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <u val="single"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF0000"/>
+        <bgColor rgb="00FF0000"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -71,26 +72,86 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+  <cellXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -356,166 +417,92 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A2:C48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.88671875" defaultRowHeight="14.4" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="26.77734375" customWidth="1"/>
-    <col min="2" max="2" width="21.109375" customWidth="1"/>
-    <col min="3" max="3" width="17.77734375" customWidth="1"/>
+    <col width="26.77734375" customWidth="1" style="2" min="1" max="1"/>
+    <col width="21.109375" customWidth="1" style="2" min="2" max="2"/>
+    <col width="17.77734375" customWidth="1" style="2" min="3" max="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
+    <row r="2">
+      <c r="A2" s="4" t="n">
         <v>1006797846</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
+    <row r="3">
+      <c r="A3" s="4" t="n">
         <v>1121872788</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2"/>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" s="2"/>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" s="2"/>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" s="2"/>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" s="2"/>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" s="2"/>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" s="2"/>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" s="2"/>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A12" s="2"/>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A13" s="2"/>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A14" s="2"/>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A15" s="2"/>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A16" s="2"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="3"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="3"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="3"/>
-      <c r="C19" s="1"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="3"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="3"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="3"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="2"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="2"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="2"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="2"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="2"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="2"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="2"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="2"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="2"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="2"/>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" s="2"/>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" s="2"/>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35" s="2"/>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A36" s="2"/>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A37" s="2"/>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A38" s="2"/>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A39" s="2"/>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A40" s="2"/>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A41" s="2"/>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A42" s="2"/>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A43" s="2"/>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A44" s="2"/>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A45" s="2"/>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A46" s="2"/>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A47" s="2"/>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A48" s="2"/>
-    </row>
+    <row r="4"/>
+    <row r="5"/>
+    <row r="6"/>
+    <row r="7"/>
+    <row r="8"/>
+    <row r="9"/>
+    <row r="10"/>
+    <row r="11"/>
+    <row r="12"/>
+    <row r="13"/>
+    <row r="14"/>
+    <row r="15"/>
+    <row r="16"/>
+    <row r="17">
+      <c r="A17" s="3" t="n"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="3" t="n"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="3" t="n"/>
+      <c r="C19" s="1" t="n"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="3" t="n"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="3" t="n"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="3" t="n"/>
+    </row>
+    <row r="23"/>
+    <row r="24"/>
+    <row r="25"/>
+    <row r="26"/>
+    <row r="27"/>
+    <row r="28"/>
+    <row r="29"/>
+    <row r="30"/>
+    <row r="31"/>
+    <row r="32"/>
+    <row r="33"/>
+    <row r="34"/>
+    <row r="35"/>
+    <row r="36"/>
+    <row r="37"/>
+    <row r="38"/>
+    <row r="39"/>
+    <row r="40"/>
+    <row r="41"/>
+    <row r="42"/>
+    <row r="43"/>
+    <row r="44"/>
+    <row r="45"/>
+    <row r="46"/>
+    <row r="47"/>
+    <row r="48"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>